<commit_message>
update protein benchmark and complex benchmark
</commit_message>
<xml_diff>
--- a/phase_02_validation/benchmark/ncaa-containing_complex.xlsx
+++ b/phase_02_validation/benchmark/ncaa-containing_complex.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5C67DF-2EA5-4A7C-B010-801608FAF3B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E42F87-42F3-4E03-8409-C74EE600DC46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="159">
   <si>
     <t>year</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -337,10 +337,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>AMOK group at C terminal for covalently and potently inhibiting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>both peptide and protein contain ncaa</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -818,6 +814,31 @@
   </si>
   <si>
     <t>10.1021/jm301674z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turning a Substrate Peptide into a Potent Inhibitor for the Histone Methyltransferase SETD8</t>
+  </si>
+  <si>
+    <t>SETD8</t>
+  </si>
+  <si>
+    <t>10.1021/acsmedchemlett.6b00303</t>
+  </si>
+  <si>
+    <t>5TEG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMOK group at C terminal, beta-aa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D-aa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NLE,etc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -825,7 +846,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -876,6 +897,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C5700"/>
       <name val="等线"/>
       <family val="2"/>
@@ -883,7 +912,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -893,6 +922,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -910,7 +944,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -918,17 +952,22 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="差" xfId="2" builtinId="27"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="好" xfId="1" builtinId="26"/>
-    <cellStyle name="适中" xfId="2" builtinId="28"/>
+    <cellStyle name="适中" xfId="3" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1206,22 +1245,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L24"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="56" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" style="1"/>
     <col min="8" max="8" width="8.88671875" style="1" customWidth="1"/>
     <col min="9" max="9" width="18.88671875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="71.21875" style="1" customWidth="1"/>
     <col min="11" max="11" width="52.6640625" style="1" customWidth="1"/>
     <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -1263,9 +1304,9 @@
         <v>2013</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1275,19 +1316,19 @@
         <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="1">
+        <v>82</v>
+      </c>
+      <c r="G2" s="3">
         <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>39</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>42</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1295,9 +1336,9 @@
         <v>2014</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1307,9 +1348,9 @@
         <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G3" s="1">
+        <v>81</v>
+      </c>
+      <c r="G3" s="3">
         <v>4</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -1319,7 +1360,7 @@
         <v>40</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>42</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1329,7 +1370,7 @@
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1345,13 +1386,13 @@
         <v>3</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
@@ -1361,7 +1402,7 @@
       <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1373,14 +1414,14 @@
       <c r="F5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="1">
-        <v>3</v>
+      <c r="G5" s="2">
+        <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1390,7 +1431,7 @@
       <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1400,7 +1441,7 @@
         <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
@@ -1419,7 +1460,7 @@
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1431,7 +1472,7 @@
       <c r="F7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="4">
         <v>2</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -1449,31 +1490,31 @@
         <v>2015</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="1">
+      <c r="G8" s="3">
         <v>4</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1481,19 +1522,19 @@
         <v>2018</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G9" s="1">
         <v>2</v>
@@ -1502,7 +1543,7 @@
         <v>30</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1510,19 +1551,19 @@
         <v>2021</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G10" s="1">
         <v>2</v>
@@ -1531,10 +1572,10 @@
         <v>30</v>
       </c>
       <c r="J10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1542,31 +1583,31 @@
         <v>2016</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G11" s="1">
         <v>3</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L11" s="1"/>
     </row>
@@ -1575,28 +1616,31 @@
         <v>2012</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G12" s="1">
-        <v>5</v>
+      <c r="G12">
+        <v>3</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="L12" s="1"/>
     </row>
@@ -1605,28 +1649,28 @@
         <v>2012</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="G13" s="1">
         <v>2</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L13" s="1"/>
     </row>
@@ -1635,31 +1679,31 @@
         <v>2009</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G14" s="1">
+        <v>138</v>
+      </c>
+      <c r="G14" s="3">
         <v>4</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1667,31 +1711,31 @@
         <v>2004</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C15" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G15" s="1">
+        <v>134</v>
+      </c>
+      <c r="G15" s="3">
         <v>4</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>30</v>
       </c>
       <c r="J15" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -1699,31 +1743,31 @@
         <v>2012</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G16" s="1">
+        <v>139</v>
+      </c>
+      <c r="G16" s="3">
         <v>4</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -1731,19 +1775,19 @@
         <v>2012</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>144</v>
+        <v>151</v>
+      </c>
+      <c r="C17" t="s">
+        <v>143</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G17" s="1">
         <v>2</v>
@@ -1752,194 +1796,222 @@
         <v>30</v>
       </c>
       <c r="J17" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>146</v>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G18" s="2">
+        <v>5</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>2016</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="G21" s="1">
         <v>0</v>
       </c>
       <c r="I21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L21" s="1"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>2011</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="G22" s="1">
         <v>0</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G23" s="1">
         <v>0</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="G24" s="1">
         <v>0</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Reselect benchmark and explore optimize strategy.
</commit_message>
<xml_diff>
--- a/phase_02_validation/benchmark/ncaa-containing_complex.xlsx
+++ b/phase_02_validation/benchmark/ncaa-containing_complex.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E42F87-42F3-4E03-8409-C74EE600DC46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E487DF9-2AEF-4933-83A2-70C2B10B0663}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="161">
   <si>
     <t>year</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -840,6 +840,13 @@
   <si>
     <t>NLE,etc</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6TCH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ultra-large chemical libraries for the discovery of high-affinity peptide binders</t>
   </si>
 </sst>
 </file>
@@ -1246,10 +1253,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1828,54 +1835,36 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K19" s="1" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>160</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K20" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>2016</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="G21" s="1">
         <v>0</v>
@@ -1883,32 +1872,26 @@
       <c r="I21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="K21" s="1" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="G22" s="1">
         <v>0</v>
@@ -1917,28 +1900,31 @@
         <v>47</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>2011</v>
+        <v>2013</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G23" s="1">
         <v>0</v>
@@ -1947,31 +1933,28 @@
         <v>47</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G24" s="1">
         <v>0</v>
@@ -1980,36 +1963,69 @@
         <v>47</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="G25" s="1">
         <v>0</v>
       </c>
       <c r="I25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>